<commit_message>
chg: Updated Syria as candidate for air attack, update road to war brief, updated situation combatflite file
</commit_message>
<xml_diff>
--- a/UNDER DEVELOPMENT/OPAR Version 2/OPAR v2.0_JOINT_TARGET_LIST.xlsx
+++ b/UNDER DEVELOPMENT/OPAR Version 2/OPAR v2.0_JOINT_TARGET_LIST.xlsx
@@ -4277,21 +4277,26 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4303,24 +4308,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4329,6 +4326,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5979,9 +5979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H124" sqref="H124"/>
+      <selection pane="topRight" activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -8774,12 +8774,14 @@
       </c>
     </row>
     <row r="116" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A116" s="177" t="s">
+      <c r="A116" s="159" t="s">
         <v>788</v>
       </c>
-      <c r="B116" s="220" t="s">
+      <c r="B116" s="186" t="s">
         <v>856</v>
       </c>
+      <c r="C116" s="187"/>
+      <c r="D116" s="187"/>
       <c r="E116" s="234" t="s">
         <v>857</v>
       </c>
@@ -8794,29 +8796,34 @@
       </c>
     </row>
     <row r="117" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A117" s="159" t="s">
+      <c r="A117" s="183" t="s">
         <v>789</v>
       </c>
-      <c r="B117" s="220" t="s">
+      <c r="B117" s="183" t="s">
         <v>862</v>
       </c>
-      <c r="E117" s="234" t="s">
+      <c r="C117" s="184"/>
+      <c r="D117" s="184"/>
+      <c r="E117" s="185" t="s">
         <v>863</v>
       </c>
-      <c r="F117" s="220" t="s">
+      <c r="F117" s="185" t="s">
         <v>864</v>
       </c>
-      <c r="G117" s="235" t="s">
+      <c r="G117" s="185" t="s">
         <v>865</v>
       </c>
+      <c r="H117" s="185"/>
     </row>
     <row r="118" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A118" s="177" t="s">
+      <c r="A118" s="159" t="s">
         <v>790</v>
       </c>
-      <c r="B118" s="216" t="s">
+      <c r="B118" s="186" t="s">
         <v>866</v>
       </c>
+      <c r="C118" s="187"/>
+      <c r="D118" s="187"/>
       <c r="E118" s="234" t="s">
         <v>867</v>
       </c>
@@ -8829,32 +8836,36 @@
       <c r="H118" s="216"/>
     </row>
     <row r="119" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A119" s="159" t="s">
+      <c r="A119" s="177" t="s">
         <v>791</v>
       </c>
-      <c r="B119" s="219" t="s">
+      <c r="B119" s="183" t="s">
         <v>870</v>
       </c>
-      <c r="E119" s="234" t="s">
+      <c r="C119" s="184"/>
+      <c r="D119" s="184"/>
+      <c r="E119" s="185" t="s">
         <v>871</v>
       </c>
-      <c r="F119" s="219" t="s">
+      <c r="F119" s="185" t="s">
         <v>872</v>
       </c>
-      <c r="G119" s="219" t="s">
+      <c r="G119" s="185" t="s">
         <v>873</v>
       </c>
-      <c r="H119" s="219" t="s">
+      <c r="H119" s="185" t="s">
         <v>861</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A120" s="177" t="s">
+      <c r="A120" s="159" t="s">
         <v>792</v>
       </c>
-      <c r="B120" s="219" t="s">
+      <c r="B120" s="186" t="s">
         <v>874</v>
       </c>
+      <c r="C120" s="187"/>
+      <c r="D120" s="187"/>
       <c r="E120" s="234" t="s">
         <v>875</v>
       </c>
@@ -8869,12 +8880,14 @@
       </c>
     </row>
     <row r="121" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A121" s="159" t="s">
+      <c r="A121" s="177" t="s">
         <v>793</v>
       </c>
-      <c r="B121" s="219" t="s">
+      <c r="B121" s="183" t="s">
         <v>878</v>
       </c>
+      <c r="C121" s="184"/>
+      <c r="D121" s="184"/>
       <c r="E121" s="234" t="s">
         <v>879</v>
       </c>
@@ -8889,12 +8902,14 @@
       </c>
     </row>
     <row r="122" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A122" s="177" t="s">
+      <c r="A122" s="159" t="s">
         <v>794</v>
       </c>
-      <c r="B122" s="219" t="s">
+      <c r="B122" s="186" t="s">
         <v>882</v>
       </c>
+      <c r="C122" s="187"/>
+      <c r="D122" s="187"/>
       <c r="E122" s="234" t="s">
         <v>883</v>
       </c>
@@ -8912,11 +8927,11 @@
       <c r="A123" s="177" t="s">
         <v>795</v>
       </c>
-      <c r="B123" s="216" t="s">
+      <c r="B123" s="183" t="s">
         <v>886</v>
       </c>
-      <c r="C123" s="232"/>
-      <c r="D123" s="232"/>
+      <c r="C123" s="184"/>
+      <c r="D123" s="184"/>
       <c r="E123" s="234" t="s">
         <v>887</v>
       </c>
@@ -15560,33 +15575,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1">
-      <c r="A1" s="256" t="s">
+      <c r="A1" s="240" t="s">
         <v>630</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="258"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
+      <c r="I1" s="242"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="259" t="s">
+      <c r="A2" s="243" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="244"/>
       <c r="C2" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="260" t="s">
+      <c r="D2" s="245" t="s">
         <v>632</v>
       </c>
-      <c r="E2" s="247"/>
-      <c r="F2" s="247"/>
+      <c r="E2" s="246"/>
+      <c r="F2" s="246"/>
       <c r="G2" s="244"/>
-      <c r="H2" s="261"/>
+      <c r="H2" s="247"/>
       <c r="I2" s="248"/>
     </row>
     <row r="3" spans="1:11">
@@ -15595,17 +15610,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75">
-      <c r="A4" s="262" t="s">
+      <c r="A4" s="249" t="s">
         <v>634</v>
       </c>
-      <c r="B4" s="257"/>
-      <c r="C4" s="257"/>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257"/>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="258"/>
+      <c r="B4" s="241"/>
+      <c r="C4" s="241"/>
+      <c r="D4" s="241"/>
+      <c r="E4" s="241"/>
+      <c r="F4" s="241"/>
+      <c r="G4" s="241"/>
+      <c r="H4" s="241"/>
+      <c r="I4" s="242"/>
     </row>
     <row r="5" spans="1:11" ht="14.25">
       <c r="A5" s="85" t="s">
@@ -15752,17 +15767,17 @@
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:11" ht="15.75">
-      <c r="A15" s="249" t="s">
+      <c r="A15" s="250" t="s">
         <v>641</v>
       </c>
-      <c r="B15" s="250"/>
-      <c r="C15" s="250"/>
-      <c r="D15" s="250"/>
-      <c r="E15" s="250"/>
-      <c r="F15" s="250"/>
-      <c r="G15" s="250"/>
-      <c r="H15" s="250"/>
-      <c r="I15" s="251"/>
+      <c r="B15" s="251"/>
+      <c r="C15" s="251"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="251"/>
+      <c r="F15" s="251"/>
+      <c r="G15" s="251"/>
+      <c r="H15" s="251"/>
+      <c r="I15" s="252"/>
     </row>
     <row r="16" spans="1:11" ht="14.25">
       <c r="A16" s="89" t="s">
@@ -15777,15 +15792,15 @@
       <c r="D16" s="90" t="s">
         <v>640</v>
       </c>
-      <c r="E16" s="252" t="s">
+      <c r="E16" s="253" t="s">
         <v>642</v>
       </c>
-      <c r="F16" s="255"/>
-      <c r="G16" s="252" t="s">
+      <c r="F16" s="256"/>
+      <c r="G16" s="253" t="s">
         <v>643</v>
       </c>
-      <c r="H16" s="253"/>
-      <c r="I16" s="254"/>
+      <c r="H16" s="254"/>
+      <c r="I16" s="255"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="91">
@@ -15794,11 +15809,11 @@
       <c r="B17" s="92"/>
       <c r="C17" s="92"/>
       <c r="D17" s="92"/>
-      <c r="E17" s="240"/>
-      <c r="F17" s="241"/>
-      <c r="G17" s="240"/>
-      <c r="H17" s="245"/>
-      <c r="I17" s="246"/>
+      <c r="E17" s="257"/>
+      <c r="F17" s="258"/>
+      <c r="G17" s="257"/>
+      <c r="H17" s="259"/>
+      <c r="I17" s="260"/>
       <c r="K17" s="84" t="s">
         <v>646</v>
       </c>
@@ -15810,11 +15825,11 @@
       <c r="B18" s="92"/>
       <c r="C18" s="92"/>
       <c r="D18" s="92"/>
-      <c r="E18" s="240"/>
-      <c r="F18" s="241"/>
-      <c r="G18" s="240"/>
-      <c r="H18" s="245"/>
-      <c r="I18" s="246"/>
+      <c r="E18" s="257"/>
+      <c r="F18" s="258"/>
+      <c r="G18" s="257"/>
+      <c r="H18" s="259"/>
+      <c r="I18" s="260"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="91">
@@ -15823,11 +15838,11 @@
       <c r="B19" s="92"/>
       <c r="C19" s="92"/>
       <c r="D19" s="92"/>
-      <c r="E19" s="240"/>
-      <c r="F19" s="241"/>
-      <c r="G19" s="240"/>
-      <c r="H19" s="245"/>
-      <c r="I19" s="246"/>
+      <c r="E19" s="257"/>
+      <c r="F19" s="258"/>
+      <c r="G19" s="257"/>
+      <c r="H19" s="259"/>
+      <c r="I19" s="260"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="91">
@@ -15836,11 +15851,11 @@
       <c r="B20" s="92"/>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
-      <c r="E20" s="240"/>
-      <c r="F20" s="241"/>
-      <c r="G20" s="240"/>
-      <c r="H20" s="245"/>
-      <c r="I20" s="246"/>
+      <c r="E20" s="257"/>
+      <c r="F20" s="258"/>
+      <c r="G20" s="257"/>
+      <c r="H20" s="259"/>
+      <c r="I20" s="260"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="91">
@@ -15849,11 +15864,11 @@
       <c r="B21" s="92"/>
       <c r="C21" s="92"/>
       <c r="D21" s="92"/>
-      <c r="E21" s="240"/>
-      <c r="F21" s="241"/>
-      <c r="G21" s="240"/>
-      <c r="H21" s="245"/>
-      <c r="I21" s="246"/>
+      <c r="E21" s="257"/>
+      <c r="F21" s="258"/>
+      <c r="G21" s="257"/>
+      <c r="H21" s="259"/>
+      <c r="I21" s="260"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="91">
@@ -15862,11 +15877,11 @@
       <c r="B22" s="92"/>
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
-      <c r="E22" s="240"/>
-      <c r="F22" s="241"/>
-      <c r="G22" s="240"/>
-      <c r="H22" s="245"/>
-      <c r="I22" s="246"/>
+      <c r="E22" s="257"/>
+      <c r="F22" s="258"/>
+      <c r="G22" s="257"/>
+      <c r="H22" s="259"/>
+      <c r="I22" s="260"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="91">
@@ -15875,11 +15890,11 @@
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
       <c r="D23" s="92"/>
-      <c r="E23" s="240"/>
-      <c r="F23" s="241"/>
-      <c r="G23" s="240"/>
-      <c r="H23" s="245"/>
-      <c r="I23" s="246"/>
+      <c r="E23" s="257"/>
+      <c r="F23" s="258"/>
+      <c r="G23" s="257"/>
+      <c r="H23" s="259"/>
+      <c r="I23" s="260"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="91">
@@ -15888,11 +15903,11 @@
       <c r="B24" s="92"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
-      <c r="E24" s="240"/>
-      <c r="F24" s="241"/>
-      <c r="G24" s="240"/>
-      <c r="H24" s="245"/>
-      <c r="I24" s="246"/>
+      <c r="E24" s="257"/>
+      <c r="F24" s="258"/>
+      <c r="G24" s="257"/>
+      <c r="H24" s="259"/>
+      <c r="I24" s="260"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="91">
@@ -15901,11 +15916,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="242"/>
-      <c r="F25" s="241"/>
-      <c r="G25" s="242"/>
-      <c r="H25" s="245"/>
-      <c r="I25" s="246"/>
+      <c r="E25" s="261"/>
+      <c r="F25" s="258"/>
+      <c r="G25" s="261"/>
+      <c r="H25" s="259"/>
+      <c r="I25" s="260"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="94">
@@ -15914,10 +15929,10 @@
       <c r="B26" s="95"/>
       <c r="C26" s="95"/>
       <c r="D26" s="95"/>
-      <c r="E26" s="243"/>
+      <c r="E26" s="262"/>
       <c r="F26" s="244"/>
-      <c r="G26" s="243"/>
-      <c r="H26" s="247"/>
+      <c r="G26" s="262"/>
+      <c r="H26" s="246"/>
       <c r="I26" s="248"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1"/>
@@ -16896,16 +16911,12 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="E19:F19"/>
@@ -16918,12 +16929,16 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="G23:I23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -16954,49 +16969,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1">
-      <c r="A1" s="256" t="s">
+      <c r="A1" s="240" t="s">
         <v>630</v>
       </c>
-      <c r="B1" s="257"/>
-      <c r="C1" s="257"/>
-      <c r="D1" s="257"/>
-      <c r="E1" s="257"/>
-      <c r="F1" s="257"/>
-      <c r="G1" s="257"/>
-      <c r="H1" s="257"/>
-      <c r="I1" s="258"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
+      <c r="I1" s="242"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="259" t="s">
+      <c r="A2" s="243" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="244"/>
       <c r="C2" s="100" t="s">
         <v>655</v>
       </c>
-      <c r="D2" s="260" t="s">
+      <c r="D2" s="245" t="s">
         <v>632</v>
       </c>
-      <c r="E2" s="247"/>
-      <c r="F2" s="247"/>
+      <c r="E2" s="246"/>
+      <c r="F2" s="246"/>
       <c r="G2" s="244"/>
-      <c r="H2" s="261" t="s">
+      <c r="H2" s="247" t="s">
         <v>656</v>
       </c>
       <c r="I2" s="248"/>
     </row>
     <row r="4" spans="1:17" ht="15.75">
-      <c r="A4" s="262" t="s">
+      <c r="A4" s="249" t="s">
         <v>634</v>
       </c>
-      <c r="B4" s="257"/>
-      <c r="C4" s="257"/>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257"/>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="258"/>
+      <c r="B4" s="241"/>
+      <c r="C4" s="241"/>
+      <c r="D4" s="241"/>
+      <c r="E4" s="241"/>
+      <c r="F4" s="241"/>
+      <c r="G4" s="241"/>
+      <c r="H4" s="241"/>
+      <c r="I4" s="242"/>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="85" t="s">
@@ -17058,15 +17073,15 @@
       <c r="I6" s="97" t="s">
         <v>664</v>
       </c>
-      <c r="K6" s="264" t="s">
+      <c r="K6" s="263" t="s">
         <v>665</v>
       </c>
-      <c r="L6" s="265"/>
-      <c r="M6" s="265"/>
-      <c r="N6" s="265"/>
-      <c r="O6" s="265"/>
-      <c r="P6" s="265"/>
-      <c r="Q6" s="265"/>
+      <c r="L6" s="264"/>
+      <c r="M6" s="264"/>
+      <c r="N6" s="264"/>
+      <c r="O6" s="264"/>
+      <c r="P6" s="264"/>
+      <c r="Q6" s="264"/>
     </row>
     <row r="7" spans="1:17" ht="14.25">
       <c r="A7" s="96">
@@ -17096,15 +17111,15 @@
       <c r="I7" s="97" t="s">
         <v>672</v>
       </c>
-      <c r="K7" s="264" t="s">
+      <c r="K7" s="263" t="s">
         <v>673</v>
       </c>
-      <c r="L7" s="265"/>
-      <c r="M7" s="265"/>
-      <c r="N7" s="265"/>
-      <c r="O7" s="265"/>
-      <c r="P7" s="265"/>
-      <c r="Q7" s="265"/>
+      <c r="L7" s="264"/>
+      <c r="M7" s="264"/>
+      <c r="N7" s="264"/>
+      <c r="O7" s="264"/>
+      <c r="P7" s="264"/>
+      <c r="Q7" s="264"/>
     </row>
     <row r="8" spans="1:17" ht="14.25">
       <c r="A8" s="96">
@@ -17212,17 +17227,17 @@
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:17" ht="15.75">
-      <c r="A15" s="249" t="s">
+      <c r="A15" s="250" t="s">
         <v>641</v>
       </c>
-      <c r="B15" s="250"/>
-      <c r="C15" s="250"/>
-      <c r="D15" s="250"/>
-      <c r="E15" s="250"/>
-      <c r="F15" s="250"/>
-      <c r="G15" s="250"/>
-      <c r="H15" s="250"/>
-      <c r="I15" s="251"/>
+      <c r="B15" s="251"/>
+      <c r="C15" s="251"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="251"/>
+      <c r="F15" s="251"/>
+      <c r="G15" s="251"/>
+      <c r="H15" s="251"/>
+      <c r="I15" s="252"/>
     </row>
     <row r="16" spans="1:17" ht="14.25">
       <c r="A16" s="85" t="s">
@@ -17237,15 +17252,15 @@
       <c r="D16" s="86" t="s">
         <v>640</v>
       </c>
-      <c r="E16" s="266" t="s">
+      <c r="E16" s="265" t="s">
         <v>642</v>
       </c>
-      <c r="F16" s="241"/>
-      <c r="G16" s="266" t="s">
+      <c r="F16" s="258"/>
+      <c r="G16" s="265" t="s">
         <v>643</v>
       </c>
-      <c r="H16" s="245"/>
-      <c r="I16" s="246"/>
+      <c r="H16" s="259"/>
+      <c r="I16" s="260"/>
     </row>
     <row r="17" spans="1:11" ht="14.25">
       <c r="A17" s="91">
@@ -17260,15 +17275,15 @@
       <c r="D17" s="88" t="s">
         <v>654</v>
       </c>
-      <c r="E17" s="263" t="s">
+      <c r="E17" s="266" t="s">
         <v>652</v>
       </c>
-      <c r="F17" s="241"/>
-      <c r="G17" s="263" t="s">
+      <c r="F17" s="258"/>
+      <c r="G17" s="266" t="s">
         <v>680</v>
       </c>
-      <c r="H17" s="245"/>
-      <c r="I17" s="246"/>
+      <c r="H17" s="259"/>
+      <c r="I17" s="260"/>
     </row>
     <row r="18" spans="1:11" ht="22.5">
       <c r="A18" s="91">
@@ -17283,15 +17298,15 @@
       <c r="D18" s="88" t="s">
         <v>654</v>
       </c>
-      <c r="E18" s="263" t="s">
+      <c r="E18" s="266" t="s">
         <v>652</v>
       </c>
-      <c r="F18" s="241"/>
-      <c r="G18" s="263" t="s">
+      <c r="F18" s="258"/>
+      <c r="G18" s="266" t="s">
         <v>681</v>
       </c>
-      <c r="H18" s="245"/>
-      <c r="I18" s="246"/>
+      <c r="H18" s="259"/>
+      <c r="I18" s="260"/>
     </row>
     <row r="19" spans="1:11" ht="34.5">
       <c r="A19" s="91">
@@ -17306,15 +17321,15 @@
       <c r="D19" s="88" t="s">
         <v>645</v>
       </c>
-      <c r="E19" s="263" t="s">
+      <c r="E19" s="266" t="s">
         <v>683</v>
       </c>
-      <c r="F19" s="241"/>
-      <c r="G19" s="263" t="s">
+      <c r="F19" s="258"/>
+      <c r="G19" s="266" t="s">
         <v>684</v>
       </c>
-      <c r="H19" s="245"/>
-      <c r="I19" s="246"/>
+      <c r="H19" s="259"/>
+      <c r="I19" s="260"/>
       <c r="K19" s="84" t="s">
         <v>646</v>
       </c>
@@ -17326,11 +17341,11 @@
       <c r="B20" s="92"/>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
-      <c r="E20" s="240"/>
-      <c r="F20" s="241"/>
-      <c r="G20" s="240"/>
-      <c r="H20" s="245"/>
-      <c r="I20" s="246"/>
+      <c r="E20" s="257"/>
+      <c r="F20" s="258"/>
+      <c r="G20" s="257"/>
+      <c r="H20" s="259"/>
+      <c r="I20" s="260"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="91">
@@ -17339,11 +17354,11 @@
       <c r="B21" s="92"/>
       <c r="C21" s="92"/>
       <c r="D21" s="92"/>
-      <c r="E21" s="240"/>
-      <c r="F21" s="241"/>
-      <c r="G21" s="240"/>
-      <c r="H21" s="245"/>
-      <c r="I21" s="246"/>
+      <c r="E21" s="257"/>
+      <c r="F21" s="258"/>
+      <c r="G21" s="257"/>
+      <c r="H21" s="259"/>
+      <c r="I21" s="260"/>
       <c r="K21" s="84" t="s">
         <v>685</v>
       </c>
@@ -17355,11 +17370,11 @@
       <c r="B22" s="92"/>
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
-      <c r="E22" s="240"/>
-      <c r="F22" s="241"/>
-      <c r="G22" s="240"/>
-      <c r="H22" s="245"/>
-      <c r="I22" s="246"/>
+      <c r="E22" s="257"/>
+      <c r="F22" s="258"/>
+      <c r="G22" s="257"/>
+      <c r="H22" s="259"/>
+      <c r="I22" s="260"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="91">
@@ -17368,11 +17383,11 @@
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
       <c r="D23" s="92"/>
-      <c r="E23" s="240"/>
-      <c r="F23" s="241"/>
-      <c r="G23" s="240"/>
-      <c r="H23" s="245"/>
-      <c r="I23" s="246"/>
+      <c r="E23" s="257"/>
+      <c r="F23" s="258"/>
+      <c r="G23" s="257"/>
+      <c r="H23" s="259"/>
+      <c r="I23" s="260"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="91">
@@ -17381,11 +17396,11 @@
       <c r="B24" s="92"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
-      <c r="E24" s="240"/>
-      <c r="F24" s="241"/>
-      <c r="G24" s="240"/>
-      <c r="H24" s="245"/>
-      <c r="I24" s="246"/>
+      <c r="E24" s="257"/>
+      <c r="F24" s="258"/>
+      <c r="G24" s="257"/>
+      <c r="H24" s="259"/>
+      <c r="I24" s="260"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="91">
@@ -17394,11 +17409,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="242"/>
-      <c r="F25" s="241"/>
-      <c r="G25" s="242"/>
-      <c r="H25" s="245"/>
-      <c r="I25" s="246"/>
+      <c r="E25" s="261"/>
+      <c r="F25" s="258"/>
+      <c r="G25" s="261"/>
+      <c r="H25" s="259"/>
+      <c r="I25" s="260"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="94">
@@ -17407,10 +17422,10 @@
       <c r="B26" s="95"/>
       <c r="C26" s="95"/>
       <c r="D26" s="95"/>
-      <c r="E26" s="243"/>
+      <c r="E26" s="262"/>
       <c r="F26" s="244"/>
-      <c r="G26" s="243"/>
-      <c r="H26" s="247"/>
+      <c r="G26" s="262"/>
+      <c r="H26" s="246"/>
       <c r="I26" s="248"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1"/>
@@ -18389,16 +18404,14 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18411,14 +18424,16 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -18449,8 +18464,8 @@
       <c r="A5" s="267" t="s">
         <v>687</v>
       </c>
-      <c r="B5" s="245"/>
-      <c r="C5" s="241"/>
+      <c r="B5" s="259"/>
+      <c r="C5" s="258"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="101" t="s">
@@ -18509,8 +18524,8 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="268"/>
-      <c r="B12" s="265"/>
-      <c r="C12" s="265"/>
+      <c r="B12" s="264"/>
+      <c r="C12" s="264"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="109"/>
@@ -19547,7 +19562,7 @@
       <c r="B2" s="269" t="s">
         <v>698</v>
       </c>
-      <c r="C2" s="241"/>
+      <c r="C2" s="258"/>
       <c r="O2" s="84" t="s">
         <v>686</v>
       </c>
@@ -20763,8 +20778,8 @@
       <c r="A3" s="269" t="s">
         <v>731</v>
       </c>
-      <c r="B3" s="245"/>
-      <c r="C3" s="241"/>
+      <c r="B3" s="259"/>
+      <c r="C3" s="258"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="101" t="s">
@@ -20773,7 +20788,7 @@
       <c r="B4" s="267" t="s">
         <v>732</v>
       </c>
-      <c r="C4" s="241"/>
+      <c r="C4" s="258"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1">
       <c r="A5" s="120" t="s">
@@ -20782,7 +20797,7 @@
       <c r="B5" s="270" t="s">
         <v>733</v>
       </c>
-      <c r="C5" s="241"/>
+      <c r="C5" s="258"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1">
       <c r="A6" s="120" t="s">
@@ -20791,7 +20806,7 @@
       <c r="B6" s="270" t="s">
         <v>734</v>
       </c>
-      <c r="C6" s="241"/>
+      <c r="C6" s="258"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1">
       <c r="A7" s="120" t="s">
@@ -20800,7 +20815,7 @@
       <c r="B7" s="270" t="s">
         <v>735</v>
       </c>
-      <c r="C7" s="241"/>
+      <c r="C7" s="258"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1">
       <c r="A8" s="120" t="s">
@@ -20809,13 +20824,13 @@
       <c r="B8" s="270" t="s">
         <v>736</v>
       </c>
-      <c r="C8" s="241"/>
+      <c r="C8" s="258"/>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="269" t="s">
         <v>698</v>
       </c>
-      <c r="C13" s="241"/>
+      <c r="C13" s="258"/>
     </row>
     <row r="14" spans="1:10" ht="15.75">
       <c r="B14" s="116" t="s">
@@ -22016,8 +22031,8 @@
       <c r="B2" s="271" t="s">
         <v>737</v>
       </c>
-      <c r="C2" s="257"/>
-      <c r="D2" s="258"/>
+      <c r="C2" s="241"/>
+      <c r="D2" s="242"/>
       <c r="J2" s="84" t="s">
         <v>686</v>
       </c>

</xml_diff>